<commit_message>
Added Last website from which I get my information from
</commit_message>
<xml_diff>
--- a/LoLChampions.xlsx
+++ b/LoLChampions.xlsx
@@ -498,11 +498,11 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1">
@@ -529,11 +529,11 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t xml:space="preserve">A </t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" ht="18.75" customHeight="1">
@@ -560,11 +560,11 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t xml:space="preserve">B </t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="18.75" customHeight="1">
@@ -591,11 +591,11 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>S</t>
+          <t xml:space="preserve">S </t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" ht="18.75" customHeight="1">
@@ -622,11 +622,11 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t xml:space="preserve">A </t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" ht="18.75" customHeight="1">
@@ -653,11 +653,11 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>B</t>
+          <t xml:space="preserve">C </t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" ht="18.75" customHeight="1">
@@ -684,11 +684,11 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>A</t>
+          <t xml:space="preserve">A </t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added adjusted values to grades
</commit_message>
<xml_diff>
--- a/LoLChampions.xlsx
+++ b/LoLChampions.xlsx
@@ -15,14 +15,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -58,13 +66,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -432,22 +457,24 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="15" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="20.42578125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="13.5703125" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
-    <col width="19" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="20.42578125" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
+    <col width="19" bestFit="1" customWidth="1" style="7" min="5" max="5"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" style="5" min="6" max="7"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" style="6" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
+    <row r="1" ht="19.5" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
           <t>Champion</t>
@@ -458,237 +485,380 @@
           <t>LoLalytics grade</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>LoLalytics grade value</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Metasrc grade</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Metasrc grade value</t>
         </is>
       </c>
+      <c r="F1" s="4" t="n"/>
+      <c r="G1" s="1" t="n"/>
+      <c r="H1" s="2" t="n"/>
     </row>
-    <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="2" t="inlineStr">
+    <row r="2" ht="19.5" customHeight="1">
+      <c r="A2" t="inlineStr">
         <is>
           <t>AATROX</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>A+</t>
         </is>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="inlineStr">
+      <c r="D2" s="8" t="n">
+        <v>1.135135135135135</v>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>S+</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">B </t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
+      <c r="G2" s="8" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="H2" s="8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>8</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>8</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.835820895522388</v>
       </c>
     </row>
-    <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  AHRI</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="n">
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> AHRI</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>A-</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8" t="n">
+        <v>0.9459459459459459</v>
+      </c>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="G3" s="8" t="n">
+        <v>1.083333333333333</v>
+      </c>
+      <c r="H3" s="8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="M3" t="n">
+        <v>1.149253731343284</v>
+      </c>
+    </row>
+    <row r="4" ht="19.5" customHeight="1">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> AKALI</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>S-</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>1.22972972972973</v>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>S+</t>
+        </is>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="G4" s="8" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="H4" s="8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>8</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.835820895522388</v>
+      </c>
+    </row>
+    <row r="5" ht="19.5" customHeight="1">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> AKSHAN</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>S</t>
         </is>
       </c>
-      <c r="E3" t="n">
+      <c r="C5" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="D5" s="8" t="n">
+        <v>1.324324324324324</v>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="H5" s="8" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>12</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
         <v>13</v>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">A </t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
+      <c r="M5" t="n">
+        <v>1.358208955223881</v>
       </c>
     </row>
-    <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> AKALI</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>S-</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>S+</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>15</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">B </t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
+    <row r="6" ht="19.5" customHeight="1">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ALISTAR</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D6" s="8" t="n">
+        <v>1.040540540540541</v>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="G6" s="8" t="n">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="H6" s="8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>8</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>11</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1.149253731343284</v>
       </c>
     </row>
-    <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> AKSHAN</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>A+</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
+    <row r="7" ht="19.5" customHeight="1">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> AMUMU</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" s="8" t="n">
+        <v>0.472972972972973</v>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="G7" s="8" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="H7" s="8" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>4</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>5</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.5223880597014926</v>
+      </c>
+    </row>
+    <row r="8" ht="19.5" customHeight="1">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> ANIVIA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>B+</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="D8" s="8" t="n">
+        <v>0.8513513513513514</v>
+      </c>
+      <c r="E8" s="3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">S </t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" ht="18.75" customHeight="1">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ALISTAR</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>A-</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
+      <c r="G8" s="8" t="n">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>8</v>
+      </c>
+      <c r="J8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
         <v>11</v>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">A </t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="18.75" customHeight="1">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> AMUMU</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="D7" s="3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>8</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">C </t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" ht="18.75" customHeight="1">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ANIVIA</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>B+</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="D8" s="3" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>11</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">A </t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
+      <c r="M8" t="n">
+        <v>1.149253731343284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>